<commit_message>
rename package to exco
</commit_message>
<xml_diff>
--- a/notebooks/quickstart/quickstart_template.xlsx
+++ b/notebooks/quickstart/quickstart_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/piti/playground/excel_comment_orm/notebooks/quickstart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DC8AB3-F3D4-5346-9608-65F37C739172}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EF3AAE-B38D-D44F-BB09-73B6451E753B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{4F7BD543-69FA-DE43-9163-FFD61F6352CC}"/>
+    <workbookView xWindow="4840" yWindow="3200" windowWidth="10000" windowHeight="8880" xr2:uid="{4F7BD543-69FA-DE43-9163-FFD61F6352CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">%%begin eco
+          <t xml:space="preserve">{{--
 </t>
         </r>
         <r>
@@ -95,7 +95,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">%%end eco
+          <t xml:space="preserve">--}}
 </t>
         </r>
       </text>
@@ -110,7 +110,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">%%begin eco
+          <t xml:space="preserve">{{--
 </t>
         </r>
         <r>
@@ -143,7 +143,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>%%end eco</t>
+          <t>--}}</t>
         </r>
         <r>
           <rPr>
@@ -186,7 +186,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">%%begin eco
+          <t xml:space="preserve">{{--
 </t>
         </r>
         <r>
@@ -216,7 +216,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>%%end eco</t>
+          <t>--}}</t>
         </r>
       </text>
     </comment>
@@ -607,7 +607,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>